<commit_message>
uploading received files prior to txt conversions
</commit_message>
<xml_diff>
--- a/submission_forms/brookhaven_college/Adjudication_Dance_Details_Brookhaven_Descant.xlsx
+++ b/submission_forms/brookhaven_college/Adjudication_Dance_Details_Brookhaven_Descant.xlsx
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'ACDA Dance Details'!$C$3:$L$63</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -22,7 +22,41 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="51">
+  <si>
+    <t>COLOUR SELECTIONS</t>
+  </si>
+  <si>
+    <t>Mid 'chest'</t>
+  </si>
+  <si>
+    <t>SL:</t>
+  </si>
+  <si>
+    <t>SR:</t>
+  </si>
+  <si>
+    <t>Low 'shin'</t>
+  </si>
+  <si>
+    <t>SOFT GOOD STAGE BACKGROUND INFORMATION (select only one):</t>
+  </si>
+  <si>
+    <t>White Cyclorama</t>
+  </si>
+  <si>
+    <t>Black Velour Curtain</t>
+  </si>
+  <si>
+    <t>OTHER TECHNICAL INFORMATION</t>
+  </si>
+  <si>
+    <t>Please describe below any scenery, stage props, musical instruments, or other non-lighting technical details that will be used in the dance. Please note that all scenery must be free-standing, and no equipment will be allowed which could damage the vinyl dance floor or other parts of the venue.</t>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
   <si>
     <t>Except where otherwise noted, this work is licensed under Creative Commons Attribution-ShareAlike 4.0.</t>
   </si>
@@ -181,36 +215,6 @@
     <t>Physical colour gel changes for each dance will be possible in the Mid 'Chest', and Low 'Shin' boom lighting fixtures only.
 The host university will provide three 'rep' sets of colour for use in boom fixtures by visiting school consisting of L201 (cool), L204 (warm), and R52 (lavender). Any other colour required must be provided by visiting school upon arrival consiting of sixteen unframed cuts at ETC Source 4 36 degree size (6.25” square).
 There will be LED colour mixing available from an overhead RGBW par wash and a cyclorama RGBA flood wash. LED colour should be specified within the lighting cue tracking sheet and will be programmed into the lighting console as part of the lighting cues.</t>
-  </si>
-  <si>
-    <t>COLOUR SELECTIONS</t>
-  </si>
-  <si>
-    <t>Mid 'chest'</t>
-  </si>
-  <si>
-    <t>SL:</t>
-  </si>
-  <si>
-    <t>SR:</t>
-  </si>
-  <si>
-    <t>Low 'shin'</t>
-  </si>
-  <si>
-    <t>SOFT GOOD STAGE BACKGROUND INFORMATION (select only one):</t>
-  </si>
-  <si>
-    <t>White Cyclorama</t>
-  </si>
-  <si>
-    <t>Black Velour Curtain</t>
-  </si>
-  <si>
-    <t>OTHER TECHNICAL INFORMATION</t>
-  </si>
-  <si>
-    <t>Please describe below any scenery, stage props, musical instruments, or other non-lighting technical details that will be used in the dance. Please note that all scenery must be free-standing, and no equipment will be allowed which could damage the vinyl dance floor or other parts of the venue.</t>
   </si>
 </sst>
 </file>
@@ -597,7 +601,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
@@ -665,6 +669,81 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -675,82 +754,10 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1170,7 +1177,7 @@
   <dimension ref="A1:AMK65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B32" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55:L60"/>
+      <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -1215,44 +1222,44 @@
     <row r="3" spans="1:14">
       <c r="A3" s="2"/>
       <c r="B3" s="11"/>
-      <c r="C3" s="56" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="56"/>
-      <c r="E3" s="57" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="57"/>
-      <c r="G3" s="58" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="58"/>
-      <c r="I3" s="58"/>
-      <c r="J3" s="58"/>
-      <c r="K3" s="58"/>
-      <c r="L3" s="58"/>
+      <c r="C3" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="36"/>
+      <c r="E3" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="37"/>
+      <c r="G3" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
       <c r="M3" s="12"/>
       <c r="N3" s="5"/>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="5"/>
       <c r="B4" s="11"/>
-      <c r="C4" s="59" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="59"/>
-      <c r="E4" s="60" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="60"/>
-      <c r="G4" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" s="61"/>
-      <c r="I4" s="61"/>
-      <c r="J4" s="61"/>
-      <c r="K4" s="61"/>
-      <c r="L4" s="61"/>
+      <c r="C4" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="39"/>
+      <c r="E4" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="40"/>
+      <c r="G4" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="41"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="41"/>
+      <c r="K4" s="41"/>
+      <c r="L4" s="41"/>
       <c r="M4" s="12"/>
       <c r="N4" s="5"/>
     </row>
@@ -1275,31 +1282,31 @@
     <row r="6" spans="1:14">
       <c r="A6" s="5"/>
       <c r="B6" s="11"/>
-      <c r="C6" s="53" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="54"/>
-      <c r="E6" s="54"/>
-      <c r="F6" s="54"/>
-      <c r="G6" s="54"/>
-      <c r="H6" s="54"/>
-      <c r="I6" s="54"/>
-      <c r="J6" s="54"/>
-      <c r="K6" s="54"/>
-      <c r="L6" s="55"/>
+      <c r="C6" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="43"/>
+      <c r="K6" s="43"/>
+      <c r="L6" s="44"/>
       <c r="M6" s="12"/>
       <c r="N6" s="5"/>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="5"/>
       <c r="B7" s="11"/>
-      <c r="C7" s="43" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
+      <c r="C7" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
       <c r="F7" s="46" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="G7" s="46"/>
       <c r="H7" s="46"/>
@@ -1324,13 +1331,13 @@
     <row r="9" spans="1:14">
       <c r="A9" s="5"/>
       <c r="B9" s="11"/>
-      <c r="C9" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
+      <c r="C9" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
       <c r="F9" s="46" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="G9" s="46"/>
       <c r="H9" s="46"/>
@@ -1355,13 +1362,13 @@
     <row r="11" spans="1:14">
       <c r="A11" s="5"/>
       <c r="B11" s="11"/>
-      <c r="C11" s="43" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
+      <c r="C11" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
       <c r="F11" s="46" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="G11" s="46"/>
       <c r="H11" s="46"/>
@@ -1391,13 +1398,13 @@
     <row r="13" spans="1:14">
       <c r="A13" s="5"/>
       <c r="B13" s="11"/>
-      <c r="C13" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
+      <c r="C13" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="45"/>
+      <c r="E13" s="45"/>
       <c r="F13" s="46" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="G13" s="46"/>
       <c r="H13" s="46"/>
@@ -1427,21 +1434,21 @@
     <row r="15" spans="1:14">
       <c r="A15" s="2"/>
       <c r="B15" s="11"/>
-      <c r="C15" s="43" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="43"/>
-      <c r="E15" s="43"/>
-      <c r="F15" s="43" t="s">
-        <v>27</v>
-      </c>
-      <c r="G15" s="43"/>
-      <c r="H15" s="62" t="s">
-        <v>5</v>
+      <c r="C15" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="45"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="45" t="s">
+        <v>38</v>
+      </c>
+      <c r="G15" s="45"/>
+      <c r="H15" s="35" t="s">
+        <v>16</v>
       </c>
       <c r="I15" s="17"/>
       <c r="J15" s="15" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="K15" s="18"/>
       <c r="M15" s="12"/>
@@ -1461,13 +1468,13 @@
     <row r="17" spans="1:14">
       <c r="A17" s="5"/>
       <c r="B17" s="11"/>
-      <c r="C17" s="43" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17" s="43"/>
-      <c r="E17" s="43"/>
+      <c r="C17" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
       <c r="F17" s="46" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="G17" s="46"/>
       <c r="H17" s="46"/>
@@ -1487,13 +1494,13 @@
     <row r="19" spans="1:14">
       <c r="A19" s="5"/>
       <c r="B19" s="11"/>
-      <c r="C19" s="43" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19" s="43"/>
-      <c r="E19" s="43"/>
+      <c r="C19" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="45"/>
+      <c r="E19" s="45"/>
       <c r="F19" s="46" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="G19" s="46"/>
       <c r="H19" s="46"/>
@@ -1523,13 +1530,13 @@
     <row r="21" spans="1:14">
       <c r="A21" s="5"/>
       <c r="B21" s="11"/>
-      <c r="C21" s="43" t="s">
-        <v>31</v>
-      </c>
-      <c r="D21" s="43"/>
-      <c r="E21" s="43"/>
+      <c r="C21" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="45"/>
+      <c r="E21" s="45"/>
       <c r="F21" s="46" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="G21" s="46"/>
       <c r="H21" s="46"/>
@@ -1549,33 +1556,33 @@
     <row r="23" spans="1:14">
       <c r="A23" s="2"/>
       <c r="B23" s="11"/>
-      <c r="C23" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="D23" s="43"/>
-      <c r="E23" s="43"/>
-      <c r="F23" s="49" t="s">
-        <v>10</v>
-      </c>
-      <c r="G23" s="49"/>
-      <c r="H23" s="49"/>
-      <c r="I23" s="49"/>
-      <c r="J23" s="49"/>
-      <c r="K23" s="49"/>
-      <c r="L23" s="49"/>
+      <c r="C23" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="G23" s="47"/>
+      <c r="H23" s="47"/>
+      <c r="I23" s="47"/>
+      <c r="J23" s="47"/>
+      <c r="K23" s="47"/>
+      <c r="L23" s="47"/>
       <c r="M23" s="12"/>
       <c r="N23" s="5"/>
     </row>
     <row r="24" spans="1:14">
       <c r="A24" s="19"/>
       <c r="B24" s="20"/>
-      <c r="F24" s="49"/>
-      <c r="G24" s="49"/>
-      <c r="H24" s="49"/>
-      <c r="I24" s="49"/>
-      <c r="J24" s="49"/>
-      <c r="K24" s="49"/>
-      <c r="L24" s="49"/>
+      <c r="F24" s="47"/>
+      <c r="G24" s="47"/>
+      <c r="H24" s="47"/>
+      <c r="I24" s="47"/>
+      <c r="J24" s="47"/>
+      <c r="K24" s="47"/>
+      <c r="L24" s="47"/>
       <c r="M24" s="21"/>
       <c r="N24" s="22"/>
     </row>
@@ -1588,31 +1595,31 @@
     <row r="26" spans="1:14">
       <c r="A26" s="19"/>
       <c r="B26" s="20"/>
-      <c r="C26" s="43" t="s">
-        <v>33</v>
-      </c>
-      <c r="D26" s="43"/>
-      <c r="E26" s="43"/>
-      <c r="F26" s="49"/>
-      <c r="G26" s="49"/>
-      <c r="H26" s="49"/>
-      <c r="I26" s="49"/>
-      <c r="J26" s="49"/>
-      <c r="K26" s="49"/>
-      <c r="L26" s="49"/>
+      <c r="C26" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="D26" s="45"/>
+      <c r="E26" s="45"/>
+      <c r="F26" s="47"/>
+      <c r="G26" s="47"/>
+      <c r="H26" s="47"/>
+      <c r="I26" s="47"/>
+      <c r="J26" s="47"/>
+      <c r="K26" s="47"/>
+      <c r="L26" s="47"/>
       <c r="M26" s="21"/>
       <c r="N26" s="22"/>
     </row>
     <row r="27" spans="1:14">
       <c r="A27" s="19"/>
       <c r="B27" s="20"/>
-      <c r="F27" s="49"/>
-      <c r="G27" s="49"/>
-      <c r="H27" s="49"/>
-      <c r="I27" s="49"/>
-      <c r="J27" s="49"/>
-      <c r="K27" s="49"/>
-      <c r="L27" s="49"/>
+      <c r="F27" s="47"/>
+      <c r="G27" s="47"/>
+      <c r="H27" s="47"/>
+      <c r="I27" s="47"/>
+      <c r="J27" s="47"/>
+      <c r="K27" s="47"/>
+      <c r="L27" s="47"/>
       <c r="M27" s="21"/>
       <c r="N27" s="22"/>
     </row>
@@ -1626,31 +1633,31 @@
     <row r="29" spans="1:14">
       <c r="A29" s="19"/>
       <c r="B29" s="20"/>
-      <c r="C29" s="50" t="s">
-        <v>34</v>
-      </c>
-      <c r="D29" s="51"/>
-      <c r="E29" s="51"/>
-      <c r="F29" s="51"/>
-      <c r="G29" s="51"/>
-      <c r="H29" s="51"/>
-      <c r="I29" s="51"/>
-      <c r="J29" s="51"/>
-      <c r="K29" s="51"/>
-      <c r="L29" s="52"/>
+      <c r="C29" s="48" t="s">
+        <v>45</v>
+      </c>
+      <c r="D29" s="49"/>
+      <c r="E29" s="49"/>
+      <c r="F29" s="49"/>
+      <c r="G29" s="49"/>
+      <c r="H29" s="49"/>
+      <c r="I29" s="49"/>
+      <c r="J29" s="49"/>
+      <c r="K29" s="49"/>
+      <c r="L29" s="50"/>
       <c r="M29" s="21"/>
       <c r="N29" s="22"/>
     </row>
     <row r="30" spans="1:14">
       <c r="A30" s="2"/>
       <c r="B30" s="11"/>
-      <c r="C30" s="45" t="s">
-        <v>35</v>
-      </c>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
+      <c r="C30" s="51" t="s">
+        <v>46</v>
+      </c>
+      <c r="D30" s="51"/>
+      <c r="E30" s="51"/>
       <c r="F30" s="46" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="G30" s="46"/>
       <c r="H30" s="46"/>
@@ -1675,24 +1682,24 @@
     <row r="32" spans="1:14">
       <c r="A32" s="2"/>
       <c r="B32" s="11"/>
-      <c r="C32" s="43" t="s">
-        <v>36</v>
-      </c>
-      <c r="D32" s="43"/>
-      <c r="E32" s="43"/>
-      <c r="F32" s="47">
+      <c r="C32" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="D32" s="45"/>
+      <c r="E32" s="45"/>
+      <c r="F32" s="52">
         <v>2145334476</v>
       </c>
-      <c r="G32" s="47"/>
+      <c r="G32" s="52"/>
       <c r="H32" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="I32" s="63" t="s">
-        <v>11</v>
-      </c>
-      <c r="J32" s="48"/>
-      <c r="K32" s="48"/>
-      <c r="L32" s="48"/>
+        <v>48</v>
+      </c>
+      <c r="I32" s="53" t="s">
+        <v>22</v>
+      </c>
+      <c r="J32" s="54"/>
+      <c r="K32" s="54"/>
+      <c r="L32" s="54"/>
       <c r="M32" s="12"/>
       <c r="N32" s="5"/>
     </row>
@@ -1710,116 +1717,116 @@
     <row r="34" spans="1:14">
       <c r="A34" s="2"/>
       <c r="B34" s="11"/>
-      <c r="C34" s="41" t="s">
-        <v>38</v>
-      </c>
-      <c r="D34" s="41"/>
-      <c r="E34" s="41"/>
-      <c r="F34" s="41"/>
-      <c r="G34" s="41"/>
-      <c r="H34" s="41"/>
-      <c r="I34" s="41"/>
-      <c r="J34" s="41"/>
-      <c r="K34" s="41"/>
-      <c r="L34" s="41"/>
+      <c r="C34" s="55" t="s">
+        <v>49</v>
+      </c>
+      <c r="D34" s="55"/>
+      <c r="E34" s="55"/>
+      <c r="F34" s="55"/>
+      <c r="G34" s="55"/>
+      <c r="H34" s="55"/>
+      <c r="I34" s="55"/>
+      <c r="J34" s="55"/>
+      <c r="K34" s="55"/>
+      <c r="L34" s="55"/>
       <c r="M34" s="12"/>
       <c r="N34" s="5"/>
     </row>
     <row r="35" spans="1:14" ht="15.75" customHeight="1">
       <c r="A35" s="2"/>
       <c r="B35" s="11"/>
-      <c r="C35" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="D35" s="44"/>
-      <c r="E35" s="44"/>
-      <c r="F35" s="44"/>
-      <c r="G35" s="44"/>
-      <c r="H35" s="44"/>
-      <c r="I35" s="44"/>
-      <c r="J35" s="44"/>
-      <c r="K35" s="44"/>
-      <c r="L35" s="44"/>
+      <c r="C35" s="56" t="s">
+        <v>50</v>
+      </c>
+      <c r="D35" s="56"/>
+      <c r="E35" s="56"/>
+      <c r="F35" s="56"/>
+      <c r="G35" s="56"/>
+      <c r="H35" s="56"/>
+      <c r="I35" s="56"/>
+      <c r="J35" s="56"/>
+      <c r="K35" s="56"/>
+      <c r="L35" s="56"/>
       <c r="M35" s="12"/>
       <c r="N35" s="5"/>
     </row>
     <row r="36" spans="1:14">
       <c r="A36" s="2"/>
       <c r="B36" s="11"/>
-      <c r="C36" s="44"/>
-      <c r="D36" s="44"/>
-      <c r="E36" s="44"/>
-      <c r="F36" s="44"/>
-      <c r="G36" s="44"/>
-      <c r="H36" s="44"/>
-      <c r="I36" s="44"/>
-      <c r="J36" s="44"/>
-      <c r="K36" s="44"/>
-      <c r="L36" s="44"/>
+      <c r="C36" s="56"/>
+      <c r="D36" s="56"/>
+      <c r="E36" s="56"/>
+      <c r="F36" s="56"/>
+      <c r="G36" s="56"/>
+      <c r="H36" s="56"/>
+      <c r="I36" s="56"/>
+      <c r="J36" s="56"/>
+      <c r="K36" s="56"/>
+      <c r="L36" s="56"/>
       <c r="M36" s="12"/>
       <c r="N36" s="5"/>
     </row>
     <row r="37" spans="1:14">
       <c r="A37" s="2"/>
       <c r="B37" s="11"/>
-      <c r="C37" s="44"/>
-      <c r="D37" s="44"/>
-      <c r="E37" s="44"/>
-      <c r="F37" s="44"/>
-      <c r="G37" s="44"/>
-      <c r="H37" s="44"/>
-      <c r="I37" s="44"/>
-      <c r="J37" s="44"/>
-      <c r="K37" s="44"/>
-      <c r="L37" s="44"/>
+      <c r="C37" s="56"/>
+      <c r="D37" s="56"/>
+      <c r="E37" s="56"/>
+      <c r="F37" s="56"/>
+      <c r="G37" s="56"/>
+      <c r="H37" s="56"/>
+      <c r="I37" s="56"/>
+      <c r="J37" s="56"/>
+      <c r="K37" s="56"/>
+      <c r="L37" s="56"/>
       <c r="M37" s="12"/>
       <c r="N37" s="5"/>
     </row>
     <row r="38" spans="1:14">
       <c r="A38" s="2"/>
       <c r="B38" s="11"/>
-      <c r="C38" s="44"/>
-      <c r="D38" s="44"/>
-      <c r="E38" s="44"/>
-      <c r="F38" s="44"/>
-      <c r="G38" s="44"/>
-      <c r="H38" s="44"/>
-      <c r="I38" s="44"/>
-      <c r="J38" s="44"/>
-      <c r="K38" s="44"/>
-      <c r="L38" s="44"/>
+      <c r="C38" s="56"/>
+      <c r="D38" s="56"/>
+      <c r="E38" s="56"/>
+      <c r="F38" s="56"/>
+      <c r="G38" s="56"/>
+      <c r="H38" s="56"/>
+      <c r="I38" s="56"/>
+      <c r="J38" s="56"/>
+      <c r="K38" s="56"/>
+      <c r="L38" s="56"/>
       <c r="M38" s="12"/>
       <c r="N38" s="5"/>
     </row>
     <row r="39" spans="1:14">
       <c r="A39" s="2"/>
       <c r="B39" s="11"/>
-      <c r="C39" s="44"/>
-      <c r="D39" s="44"/>
-      <c r="E39" s="44"/>
-      <c r="F39" s="44"/>
-      <c r="G39" s="44"/>
-      <c r="H39" s="44"/>
-      <c r="I39" s="44"/>
-      <c r="J39" s="44"/>
-      <c r="K39" s="44"/>
-      <c r="L39" s="44"/>
+      <c r="C39" s="56"/>
+      <c r="D39" s="56"/>
+      <c r="E39" s="56"/>
+      <c r="F39" s="56"/>
+      <c r="G39" s="56"/>
+      <c r="H39" s="56"/>
+      <c r="I39" s="56"/>
+      <c r="J39" s="56"/>
+      <c r="K39" s="56"/>
+      <c r="L39" s="56"/>
       <c r="M39" s="12"/>
       <c r="N39" s="5"/>
     </row>
     <row r="40" spans="1:14">
       <c r="A40" s="2"/>
       <c r="B40" s="11"/>
-      <c r="C40" s="44"/>
-      <c r="D40" s="44"/>
-      <c r="E40" s="44"/>
-      <c r="F40" s="44"/>
-      <c r="G40" s="44"/>
-      <c r="H40" s="44"/>
-      <c r="I40" s="44"/>
-      <c r="J40" s="44"/>
-      <c r="K40" s="44"/>
-      <c r="L40" s="44"/>
+      <c r="C40" s="56"/>
+      <c r="D40" s="56"/>
+      <c r="E40" s="56"/>
+      <c r="F40" s="56"/>
+      <c r="G40" s="56"/>
+      <c r="H40" s="56"/>
+      <c r="I40" s="56"/>
+      <c r="J40" s="56"/>
+      <c r="K40" s="56"/>
+      <c r="L40" s="56"/>
       <c r="M40" s="12"/>
       <c r="N40" s="5"/>
     </row>
@@ -1842,42 +1849,42 @@
     <row r="42" spans="1:14">
       <c r="A42" s="2"/>
       <c r="B42" s="11"/>
-      <c r="C42" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="D42" s="41"/>
-      <c r="E42" s="41"/>
-      <c r="F42" s="41"/>
-      <c r="G42" s="41"/>
-      <c r="H42" s="41"/>
-      <c r="I42" s="41"/>
-      <c r="J42" s="41"/>
-      <c r="K42" s="41"/>
-      <c r="L42" s="41"/>
+      <c r="C42" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="D42" s="55"/>
+      <c r="E42" s="55"/>
+      <c r="F42" s="55"/>
+      <c r="G42" s="55"/>
+      <c r="H42" s="55"/>
+      <c r="I42" s="55"/>
+      <c r="J42" s="55"/>
+      <c r="K42" s="55"/>
+      <c r="L42" s="55"/>
       <c r="M42" s="12"/>
       <c r="N42" s="5"/>
     </row>
     <row r="43" spans="1:14">
       <c r="A43" s="2"/>
       <c r="B43" s="11"/>
-      <c r="C43" s="38" t="s">
-        <v>41</v>
-      </c>
-      <c r="D43" s="38"/>
+      <c r="C43" s="57" t="s">
+        <v>1</v>
+      </c>
+      <c r="D43" s="57"/>
       <c r="E43" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="F43" s="40" t="s">
-        <v>13</v>
-      </c>
-      <c r="G43" s="40"/>
+        <v>2</v>
+      </c>
+      <c r="F43" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="G43" s="58"/>
       <c r="H43" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="I43" s="40" t="s">
-        <v>13</v>
-      </c>
-      <c r="J43" s="40"/>
+        <v>3</v>
+      </c>
+      <c r="I43" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="J43" s="58"/>
       <c r="M43" s="12"/>
       <c r="N43" s="5"/>
     </row>
@@ -1891,24 +1898,24 @@
     <row r="45" spans="1:14">
       <c r="A45" s="2"/>
       <c r="B45" s="11"/>
-      <c r="C45" s="38" t="s">
-        <v>44</v>
-      </c>
-      <c r="D45" s="38"/>
+      <c r="C45" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="D45" s="57"/>
       <c r="E45" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="F45" s="40" t="s">
-        <v>12</v>
-      </c>
-      <c r="G45" s="40"/>
+        <v>2</v>
+      </c>
+      <c r="F45" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="G45" s="58"/>
       <c r="H45" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="I45" s="40" t="s">
-        <v>12</v>
-      </c>
-      <c r="J45" s="40"/>
+        <v>3</v>
+      </c>
+      <c r="I45" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="J45" s="58"/>
       <c r="M45" s="12"/>
       <c r="N45" s="5"/>
     </row>
@@ -1926,18 +1933,18 @@
     <row r="47" spans="1:14">
       <c r="A47" s="2"/>
       <c r="B47" s="11"/>
-      <c r="C47" s="41" t="s">
-        <v>45</v>
-      </c>
-      <c r="D47" s="41"/>
-      <c r="E47" s="41"/>
-      <c r="F47" s="41"/>
-      <c r="G47" s="41"/>
-      <c r="H47" s="41"/>
-      <c r="I47" s="41"/>
-      <c r="J47" s="41"/>
-      <c r="K47" s="41"/>
-      <c r="L47" s="41"/>
+      <c r="C47" s="55" t="s">
+        <v>5</v>
+      </c>
+      <c r="D47" s="55"/>
+      <c r="E47" s="55"/>
+      <c r="F47" s="55"/>
+      <c r="G47" s="55"/>
+      <c r="H47" s="55"/>
+      <c r="I47" s="55"/>
+      <c r="J47" s="55"/>
+      <c r="K47" s="55"/>
+      <c r="L47" s="55"/>
       <c r="M47" s="12"/>
       <c r="N47" s="5"/>
     </row>
@@ -1945,15 +1952,17 @@
       <c r="A48" s="19"/>
       <c r="B48" s="20"/>
       <c r="C48" s="26"/>
-      <c r="D48" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="E48" s="42"/>
-      <c r="F48" s="27"/>
-      <c r="G48" s="43" t="s">
-        <v>47</v>
-      </c>
-      <c r="H48" s="43"/>
+      <c r="D48" s="59" t="s">
+        <v>6</v>
+      </c>
+      <c r="E48" s="59"/>
+      <c r="F48" s="64" t="s">
+        <v>10</v>
+      </c>
+      <c r="G48" s="45" t="s">
+        <v>7</v>
+      </c>
+      <c r="H48" s="45"/>
       <c r="I48" s="27"/>
       <c r="M48" s="21"/>
       <c r="N48" s="22"/>
@@ -1972,13 +1981,13 @@
     <row r="50" spans="1:14" ht="15.75" customHeight="1">
       <c r="A50" s="2"/>
       <c r="B50" s="11"/>
-      <c r="C50" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="D50" s="35"/>
-      <c r="E50" s="35"/>
-      <c r="F50" s="35"/>
-      <c r="G50" s="35"/>
+      <c r="C50" s="60" t="s">
+        <v>8</v>
+      </c>
+      <c r="D50" s="60"/>
+      <c r="E50" s="60"/>
+      <c r="F50" s="60"/>
+      <c r="G50" s="60"/>
       <c r="H50" s="28"/>
       <c r="I50" s="29"/>
       <c r="J50" s="29"/>
@@ -1990,50 +1999,50 @@
     <row r="51" spans="1:14" ht="15.75" customHeight="1">
       <c r="A51" s="2"/>
       <c r="B51" s="11"/>
-      <c r="C51" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="D51" s="36"/>
-      <c r="E51" s="36"/>
-      <c r="F51" s="36"/>
-      <c r="G51" s="36"/>
-      <c r="H51" s="36"/>
-      <c r="I51" s="36"/>
-      <c r="J51" s="36"/>
-      <c r="K51" s="36"/>
-      <c r="L51" s="36"/>
+      <c r="C51" s="61" t="s">
+        <v>9</v>
+      </c>
+      <c r="D51" s="61"/>
+      <c r="E51" s="61"/>
+      <c r="F51" s="61"/>
+      <c r="G51" s="61"/>
+      <c r="H51" s="61"/>
+      <c r="I51" s="61"/>
+      <c r="J51" s="61"/>
+      <c r="K51" s="61"/>
+      <c r="L51" s="61"/>
       <c r="M51" s="12"/>
       <c r="N51" s="5"/>
     </row>
     <row r="52" spans="1:14">
       <c r="A52" s="2"/>
       <c r="B52" s="11"/>
-      <c r="C52" s="36"/>
-      <c r="D52" s="36"/>
-      <c r="E52" s="36"/>
-      <c r="F52" s="36"/>
-      <c r="G52" s="36"/>
-      <c r="H52" s="36"/>
-      <c r="I52" s="36"/>
-      <c r="J52" s="36"/>
-      <c r="K52" s="36"/>
-      <c r="L52" s="36"/>
+      <c r="C52" s="61"/>
+      <c r="D52" s="61"/>
+      <c r="E52" s="61"/>
+      <c r="F52" s="61"/>
+      <c r="G52" s="61"/>
+      <c r="H52" s="61"/>
+      <c r="I52" s="61"/>
+      <c r="J52" s="61"/>
+      <c r="K52" s="61"/>
+      <c r="L52" s="61"/>
       <c r="M52" s="12"/>
       <c r="N52" s="23"/>
     </row>
     <row r="53" spans="1:14">
       <c r="A53" s="2"/>
       <c r="B53" s="11"/>
-      <c r="C53" s="36"/>
-      <c r="D53" s="36"/>
-      <c r="E53" s="36"/>
-      <c r="F53" s="36"/>
-      <c r="G53" s="36"/>
-      <c r="H53" s="36"/>
-      <c r="I53" s="36"/>
-      <c r="J53" s="36"/>
-      <c r="K53" s="36"/>
-      <c r="L53" s="36"/>
+      <c r="C53" s="61"/>
+      <c r="D53" s="61"/>
+      <c r="E53" s="61"/>
+      <c r="F53" s="61"/>
+      <c r="G53" s="61"/>
+      <c r="H53" s="61"/>
+      <c r="I53" s="61"/>
+      <c r="J53" s="61"/>
+      <c r="K53" s="61"/>
+      <c r="L53" s="61"/>
       <c r="M53" s="12"/>
       <c r="N53" s="5"/>
     </row>
@@ -2051,98 +2060,98 @@
     <row r="55" spans="1:14" ht="15.75" customHeight="1">
       <c r="A55" s="2"/>
       <c r="B55" s="11"/>
-      <c r="C55" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="D55" s="37"/>
-      <c r="E55" s="37"/>
-      <c r="F55" s="37"/>
-      <c r="G55" s="37"/>
-      <c r="H55" s="37"/>
-      <c r="I55" s="37"/>
-      <c r="J55" s="37"/>
-      <c r="K55" s="37"/>
-      <c r="L55" s="37"/>
+      <c r="C55" s="62" t="s">
+        <v>25</v>
+      </c>
+      <c r="D55" s="62"/>
+      <c r="E55" s="62"/>
+      <c r="F55" s="62"/>
+      <c r="G55" s="62"/>
+      <c r="H55" s="62"/>
+      <c r="I55" s="62"/>
+      <c r="J55" s="62"/>
+      <c r="K55" s="62"/>
+      <c r="L55" s="62"/>
       <c r="M55" s="12"/>
       <c r="N55" s="5"/>
     </row>
     <row r="56" spans="1:14">
       <c r="A56" s="2"/>
       <c r="B56" s="11"/>
-      <c r="C56" s="37"/>
-      <c r="D56" s="37"/>
-      <c r="E56" s="37"/>
-      <c r="F56" s="37"/>
-      <c r="G56" s="37"/>
-      <c r="H56" s="37"/>
-      <c r="I56" s="37"/>
-      <c r="J56" s="37"/>
-      <c r="K56" s="37"/>
-      <c r="L56" s="37"/>
+      <c r="C56" s="62"/>
+      <c r="D56" s="62"/>
+      <c r="E56" s="62"/>
+      <c r="F56" s="62"/>
+      <c r="G56" s="62"/>
+      <c r="H56" s="62"/>
+      <c r="I56" s="62"/>
+      <c r="J56" s="62"/>
+      <c r="K56" s="62"/>
+      <c r="L56" s="62"/>
       <c r="M56" s="12"/>
       <c r="N56" s="23"/>
     </row>
     <row r="57" spans="1:14">
       <c r="A57" s="2"/>
       <c r="B57" s="11"/>
-      <c r="C57" s="37"/>
-      <c r="D57" s="37"/>
-      <c r="E57" s="37"/>
-      <c r="F57" s="37"/>
-      <c r="G57" s="37"/>
-      <c r="H57" s="37"/>
-      <c r="I57" s="37"/>
-      <c r="J57" s="37"/>
-      <c r="K57" s="37"/>
-      <c r="L57" s="37"/>
+      <c r="C57" s="62"/>
+      <c r="D57" s="62"/>
+      <c r="E57" s="62"/>
+      <c r="F57" s="62"/>
+      <c r="G57" s="62"/>
+      <c r="H57" s="62"/>
+      <c r="I57" s="62"/>
+      <c r="J57" s="62"/>
+      <c r="K57" s="62"/>
+      <c r="L57" s="62"/>
       <c r="M57" s="12"/>
       <c r="N57" s="5"/>
     </row>
     <row r="58" spans="1:14">
       <c r="A58" s="2"/>
       <c r="B58" s="11"/>
-      <c r="C58" s="37"/>
-      <c r="D58" s="37"/>
-      <c r="E58" s="37"/>
-      <c r="F58" s="37"/>
-      <c r="G58" s="37"/>
-      <c r="H58" s="37"/>
-      <c r="I58" s="37"/>
-      <c r="J58" s="37"/>
-      <c r="K58" s="37"/>
-      <c r="L58" s="37"/>
+      <c r="C58" s="62"/>
+      <c r="D58" s="62"/>
+      <c r="E58" s="62"/>
+      <c r="F58" s="62"/>
+      <c r="G58" s="62"/>
+      <c r="H58" s="62"/>
+      <c r="I58" s="62"/>
+      <c r="J58" s="62"/>
+      <c r="K58" s="62"/>
+      <c r="L58" s="62"/>
       <c r="M58" s="12"/>
       <c r="N58" s="5"/>
     </row>
     <row r="59" spans="1:14">
       <c r="A59" s="2"/>
       <c r="B59" s="11"/>
-      <c r="C59" s="37"/>
-      <c r="D59" s="37"/>
-      <c r="E59" s="37"/>
-      <c r="F59" s="37"/>
-      <c r="G59" s="37"/>
-      <c r="H59" s="37"/>
-      <c r="I59" s="37"/>
-      <c r="J59" s="37"/>
-      <c r="K59" s="37"/>
-      <c r="L59" s="37"/>
+      <c r="C59" s="62"/>
+      <c r="D59" s="62"/>
+      <c r="E59" s="62"/>
+      <c r="F59" s="62"/>
+      <c r="G59" s="62"/>
+      <c r="H59" s="62"/>
+      <c r="I59" s="62"/>
+      <c r="J59" s="62"/>
+      <c r="K59" s="62"/>
+      <c r="L59" s="62"/>
       <c r="M59" s="12"/>
       <c r="N59" s="5"/>
     </row>
     <row r="60" spans="1:14">
       <c r="A60" s="2"/>
       <c r="B60" s="11"/>
-      <c r="C60" s="37"/>
-      <c r="D60" s="37"/>
-      <c r="E60" s="37"/>
-      <c r="F60" s="37"/>
-      <c r="G60" s="37"/>
-      <c r="H60" s="37"/>
-      <c r="I60" s="37"/>
-      <c r="J60" s="37"/>
-      <c r="K60" s="37"/>
-      <c r="L60" s="37"/>
+      <c r="C60" s="62"/>
+      <c r="D60" s="62"/>
+      <c r="E60" s="62"/>
+      <c r="F60" s="62"/>
+      <c r="G60" s="62"/>
+      <c r="H60" s="62"/>
+      <c r="I60" s="62"/>
+      <c r="J60" s="62"/>
+      <c r="K60" s="62"/>
+      <c r="L60" s="62"/>
       <c r="M60" s="12"/>
       <c r="N60" s="5"/>
     </row>
@@ -2155,36 +2164,36 @@
     <row r="62" spans="1:14">
       <c r="A62" s="2"/>
       <c r="B62" s="11"/>
-      <c r="C62" s="38"/>
-      <c r="D62" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="E62" s="39"/>
-      <c r="F62" s="39"/>
-      <c r="G62" s="39"/>
-      <c r="H62" s="39"/>
-      <c r="I62" s="39"/>
-      <c r="J62" s="39"/>
-      <c r="K62" s="39"/>
-      <c r="L62" s="39"/>
+      <c r="C62" s="57"/>
+      <c r="D62" s="63" t="s">
+        <v>11</v>
+      </c>
+      <c r="E62" s="63"/>
+      <c r="F62" s="63"/>
+      <c r="G62" s="63"/>
+      <c r="H62" s="63"/>
+      <c r="I62" s="63"/>
+      <c r="J62" s="63"/>
+      <c r="K62" s="63"/>
+      <c r="L62" s="63"/>
       <c r="M62" s="12"/>
       <c r="N62" s="5"/>
     </row>
     <row r="63" spans="1:14">
       <c r="A63" s="2"/>
       <c r="B63" s="11"/>
-      <c r="C63" s="38"/>
-      <c r="D63" s="39" t="s">
-        <v>1</v>
-      </c>
-      <c r="E63" s="39"/>
-      <c r="F63" s="39"/>
-      <c r="G63" s="39"/>
-      <c r="H63" s="39"/>
-      <c r="I63" s="39"/>
-      <c r="J63" s="39"/>
-      <c r="K63" s="39"/>
-      <c r="L63" s="39"/>
+      <c r="C63" s="57"/>
+      <c r="D63" s="63" t="s">
+        <v>12</v>
+      </c>
+      <c r="E63" s="63"/>
+      <c r="F63" s="63"/>
+      <c r="G63" s="63"/>
+      <c r="H63" s="63"/>
+      <c r="I63" s="63"/>
+      <c r="J63" s="63"/>
+      <c r="K63" s="63"/>
+      <c r="L63" s="63"/>
       <c r="M63" s="12"/>
       <c r="N63" s="23"/>
     </row>
@@ -2222,57 +2231,57 @@
     </row>
   </sheetData>
   <mergeCells count="51">
+    <mergeCell ref="C50:G50"/>
+    <mergeCell ref="C51:L53"/>
+    <mergeCell ref="C55:L60"/>
+    <mergeCell ref="C62:C63"/>
+    <mergeCell ref="D62:L62"/>
+    <mergeCell ref="D63:L63"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="I45:J45"/>
+    <mergeCell ref="C47:L47"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="C34:L34"/>
+    <mergeCell ref="C35:L40"/>
+    <mergeCell ref="C42:L42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="I43:J43"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="F30:L30"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="I32:L32"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="F23:L24"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="F26:L27"/>
+    <mergeCell ref="C29:L29"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="F17:L17"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="F19:L19"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="F21:L21"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="F11:L11"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="F13:L13"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="C6:L6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="F7:L7"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="F9:L9"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="G3:L3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="G4:L4"/>
-    <mergeCell ref="C6:L6"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="F7:L7"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="F9:L9"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="F11:L11"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="F13:L13"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="F17:L17"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="F19:L19"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="F21:L21"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="F23:L24"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="F26:L27"/>
-    <mergeCell ref="C29:L29"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="F30:L30"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="I32:L32"/>
-    <mergeCell ref="C34:L34"/>
-    <mergeCell ref="C35:L40"/>
-    <mergeCell ref="C42:L42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="I43:J43"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="I45:J45"/>
-    <mergeCell ref="C47:L47"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="G48:H48"/>
-    <mergeCell ref="C50:G50"/>
-    <mergeCell ref="C51:L53"/>
-    <mergeCell ref="C55:L60"/>
-    <mergeCell ref="C62:C63"/>
-    <mergeCell ref="D62:L62"/>
-    <mergeCell ref="D63:L63"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <hyperlinks>

</xml_diff>